<commit_message>
intiialize project and add WorldReader
</commit_message>
<xml_diff>
--- a/Editorの仕様書.xlsx
+++ b/Editorの仕様書.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwuser.DA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwuser.DA\Desktop\Aether\AetherEditor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1116,6 +1116,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1123,6 +1129,183 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="7" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="6" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1144,189 +1327,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="3" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="12" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="12" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="4" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="8" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="9" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="12" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="5" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="13" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="13" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="9" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1766,10 +1766,10 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="76"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="27"/>
       <c r="E1" s="33"/>
       <c r="F1" s="33"/>
@@ -1784,17 +1784,17 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="36"/>
-      <c r="I2" s="36"/>
-      <c r="J2" s="37"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="39"/>
       <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
@@ -1810,33 +1810,33 @@
       <c r="O2" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="P2" s="80" t="s">
+      <c r="P2" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="81"/>
+      <c r="Q2" s="54"/>
       <c r="R2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S2" s="77" t="s">
+      <c r="S2" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="78"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="37"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="39"/>
       <c r="K3" s="18" t="s">
         <v>6</v>
       </c>
@@ -1852,33 +1852,33 @@
       <c r="O3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="82" t="s">
+      <c r="P3" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="83"/>
+      <c r="Q3" s="49"/>
       <c r="R3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="S3" s="79" t="s">
+      <c r="S3" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="T3" s="78"/>
+      <c r="T3" s="43"/>
     </row>
     <row r="4" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="39"/>
       <c r="K4" s="11" t="s">
         <v>6</v>
       </c>
@@ -1894,33 +1894,33 @@
       <c r="O4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="P4" s="105" t="s">
+      <c r="P4" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="Q4" s="91"/>
+      <c r="Q4" s="47"/>
       <c r="R4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="79" t="s">
+      <c r="S4" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="T4" s="78"/>
+      <c r="T4" s="43"/>
     </row>
     <row r="5" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="38" t="s">
+      <c r="B5" s="99" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="40"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="100"/>
+      <c r="I5" s="100"/>
+      <c r="J5" s="101"/>
       <c r="K5" s="18" t="s">
         <v>6</v>
       </c>
@@ -1936,33 +1936,33 @@
       <c r="O5" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P5" s="82" t="s">
+      <c r="P5" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="83"/>
+      <c r="Q5" s="49"/>
       <c r="R5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="S5" s="103" t="s">
+      <c r="S5" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="T5" s="104"/>
+      <c r="T5" s="45"/>
     </row>
     <row r="6" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="37"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="39"/>
       <c r="K6" s="14" t="s">
         <v>6</v>
       </c>
@@ -1978,33 +1978,33 @@
       <c r="O6" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P6" s="82" t="s">
+      <c r="P6" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="83"/>
+      <c r="Q6" s="49"/>
       <c r="R6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S6" s="79" t="s">
+      <c r="S6" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="T6" s="78"/>
+      <c r="T6" s="43"/>
     </row>
     <row r="7" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="39"/>
       <c r="K7" s="14" t="s">
         <v>6</v>
       </c>
@@ -2020,97 +2020,97 @@
       <c r="O7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="82" t="s">
+      <c r="P7" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="Q7" s="83"/>
+      <c r="Q7" s="49"/>
       <c r="R7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S7" s="79" t="s">
+      <c r="S7" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="T7" s="78"/>
+      <c r="T7" s="43"/>
     </row>
     <row r="8" spans="1:24" ht="13.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="57" t="s">
+      <c r="A8" s="83" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="102" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="43"/>
+      <c r="C8" s="103"/>
+      <c r="D8" s="103"/>
+      <c r="E8" s="103"/>
+      <c r="F8" s="103"/>
+      <c r="G8" s="103"/>
+      <c r="H8" s="103"/>
+      <c r="I8" s="103"/>
+      <c r="J8" s="104"/>
       <c r="K8" s="93" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="95" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="99" t="s">
+      <c r="M8" s="35" t="s">
         <v>5</v>
       </c>
       <c r="N8" s="97" t="s">
         <v>4</v>
       </c>
-      <c r="O8" s="101" t="s">
+      <c r="O8" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="P8" s="90" t="s">
+      <c r="P8" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="91"/>
-      <c r="R8" s="101" t="s">
+      <c r="Q8" s="47"/>
+      <c r="R8" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="S8" s="84" t="s">
+      <c r="S8" s="85" t="s">
         <v>21</v>
       </c>
-      <c r="T8" s="85"/>
+      <c r="T8" s="86"/>
     </row>
     <row r="9" spans="1:24" ht="43.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="58"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
+      <c r="A9" s="84"/>
+      <c r="B9" s="105"/>
+      <c r="C9" s="103"/>
+      <c r="D9" s="103"/>
+      <c r="E9" s="103"/>
+      <c r="F9" s="103"/>
+      <c r="G9" s="103"/>
+      <c r="H9" s="103"/>
+      <c r="I9" s="103"/>
+      <c r="J9" s="104"/>
       <c r="K9" s="94"/>
       <c r="L9" s="96"/>
-      <c r="M9" s="100"/>
+      <c r="M9" s="36"/>
       <c r="N9" s="98"/>
-      <c r="O9" s="102"/>
+      <c r="O9" s="41"/>
       <c r="P9" s="92"/>
-      <c r="Q9" s="91"/>
-      <c r="R9" s="102"/>
-      <c r="S9" s="86"/>
-      <c r="T9" s="85"/>
+      <c r="Q9" s="47"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="87"/>
+      <c r="T9" s="86"/>
     </row>
     <row r="10" spans="1:24" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="35" t="s">
+      <c r="B10" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="36"/>
-      <c r="F10" s="36"/>
-      <c r="G10" s="36"/>
-      <c r="H10" s="36"/>
-      <c r="I10" s="36"/>
-      <c r="J10" s="37"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="38"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="39"/>
       <c r="K10" s="14" t="s">
         <v>6</v>
       </c>
@@ -2126,29 +2126,29 @@
       <c r="O10" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="82" t="s">
+      <c r="P10" s="48" t="s">
         <v>26</v>
       </c>
-      <c r="Q10" s="83"/>
+      <c r="Q10" s="49"/>
       <c r="R10" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S10" s="79" t="s">
+      <c r="S10" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="T10" s="78"/>
+      <c r="T10" s="43"/>
     </row>
     <row r="11" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="87" t="s">
+      <c r="B11" s="88" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="88"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="89"/>
+      <c r="C11" s="89"/>
+      <c r="D11" s="89"/>
+      <c r="E11" s="89"/>
+      <c r="F11" s="90"/>
       <c r="H11" s="33"/>
       <c r="I11" s="33"/>
       <c r="J11" s="33"/>
@@ -2169,349 +2169,349 @@
       <c r="A12" s="1">
         <v>0</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="47"/>
+      <c r="C12" s="72"/>
+      <c r="D12" s="72"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
       <c r="G12" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="48" t="s">
+      <c r="H12" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I12" s="49"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="49"/>
-      <c r="L12" s="50"/>
+      <c r="I12" s="75"/>
+      <c r="J12" s="75"/>
+      <c r="K12" s="75"/>
+      <c r="L12" s="76"/>
       <c r="M12" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N12" s="51" t="s">
+      <c r="N12" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O12" s="52"/>
-      <c r="P12" s="52"/>
-      <c r="Q12" s="52"/>
-      <c r="R12" s="53"/>
+      <c r="O12" s="78"/>
+      <c r="P12" s="78"/>
+      <c r="Q12" s="78"/>
+      <c r="R12" s="79"/>
       <c r="S12" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T12" s="54" t="s">
+      <c r="T12" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U12" s="55"/>
-      <c r="V12" s="55"/>
-      <c r="W12" s="55"/>
-      <c r="X12" s="56"/>
+      <c r="U12" s="81"/>
+      <c r="V12" s="81"/>
+      <c r="W12" s="81"/>
+      <c r="X12" s="82"/>
     </row>
     <row r="13" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>1</v>
       </c>
-      <c r="B13" s="45" t="s">
+      <c r="B13" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="47"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="73"/>
       <c r="G13" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="48" t="s">
+      <c r="H13" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I13" s="49"/>
-      <c r="J13" s="49"/>
-      <c r="K13" s="49"/>
-      <c r="L13" s="50"/>
+      <c r="I13" s="75"/>
+      <c r="J13" s="75"/>
+      <c r="K13" s="75"/>
+      <c r="L13" s="76"/>
       <c r="M13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N13" s="51" t="s">
+      <c r="N13" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="52"/>
-      <c r="P13" s="52"/>
-      <c r="Q13" s="52"/>
-      <c r="R13" s="53"/>
+      <c r="O13" s="78"/>
+      <c r="P13" s="78"/>
+      <c r="Q13" s="78"/>
+      <c r="R13" s="79"/>
       <c r="S13" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T13" s="54" t="s">
+      <c r="T13" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U13" s="55"/>
-      <c r="V13" s="55"/>
-      <c r="W13" s="55"/>
-      <c r="X13" s="56"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="81"/>
+      <c r="W13" s="81"/>
+      <c r="X13" s="82"/>
     </row>
     <row r="14" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>2</v>
       </c>
-      <c r="B14" s="45" t="s">
+      <c r="B14" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="46"/>
-      <c r="D14" s="46"/>
-      <c r="E14" s="46"/>
-      <c r="F14" s="47"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
       <c r="G14" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="48" t="s">
+      <c r="H14" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="49"/>
-      <c r="J14" s="49"/>
-      <c r="K14" s="49"/>
-      <c r="L14" s="50"/>
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="K14" s="75"/>
+      <c r="L14" s="76"/>
       <c r="M14" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N14" s="51" t="s">
+      <c r="N14" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O14" s="52"/>
-      <c r="P14" s="52"/>
-      <c r="Q14" s="52"/>
-      <c r="R14" s="53"/>
+      <c r="O14" s="78"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="78"/>
+      <c r="R14" s="79"/>
       <c r="S14" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T14" s="54" t="s">
+      <c r="T14" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U14" s="55"/>
-      <c r="V14" s="55"/>
-      <c r="W14" s="55"/>
-      <c r="X14" s="56"/>
+      <c r="U14" s="81"/>
+      <c r="V14" s="81"/>
+      <c r="W14" s="81"/>
+      <c r="X14" s="82"/>
     </row>
     <row r="15" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>3</v>
       </c>
-      <c r="B15" s="45" t="s">
+      <c r="B15" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="46"/>
-      <c r="D15" s="46"/>
-      <c r="E15" s="46"/>
-      <c r="F15" s="47"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="73"/>
       <c r="G15" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="48" t="s">
+      <c r="H15" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="49"/>
-      <c r="J15" s="49"/>
-      <c r="K15" s="49"/>
-      <c r="L15" s="50"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="K15" s="75"/>
+      <c r="L15" s="76"/>
       <c r="M15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N15" s="51" t="s">
+      <c r="N15" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O15" s="52"/>
-      <c r="P15" s="52"/>
-      <c r="Q15" s="52"/>
-      <c r="R15" s="53"/>
+      <c r="O15" s="78"/>
+      <c r="P15" s="78"/>
+      <c r="Q15" s="78"/>
+      <c r="R15" s="79"/>
       <c r="S15" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T15" s="54" t="s">
+      <c r="T15" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U15" s="55"/>
-      <c r="V15" s="55"/>
-      <c r="W15" s="55"/>
-      <c r="X15" s="56"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="81"/>
+      <c r="W15" s="81"/>
+      <c r="X15" s="82"/>
     </row>
     <row r="16" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B16" s="45" t="s">
+      <c r="B16" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="46"/>
-      <c r="D16" s="46"/>
-      <c r="E16" s="46"/>
-      <c r="F16" s="47"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="73"/>
       <c r="G16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="48" t="s">
+      <c r="H16" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I16" s="49"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="49"/>
-      <c r="L16" s="50"/>
+      <c r="I16" s="75"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="75"/>
+      <c r="L16" s="76"/>
       <c r="M16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N16" s="51" t="s">
+      <c r="N16" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O16" s="52"/>
-      <c r="P16" s="52"/>
-      <c r="Q16" s="52"/>
-      <c r="R16" s="53"/>
+      <c r="O16" s="78"/>
+      <c r="P16" s="78"/>
+      <c r="Q16" s="78"/>
+      <c r="R16" s="79"/>
       <c r="S16" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T16" s="54" t="s">
+      <c r="T16" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U16" s="55"/>
-      <c r="V16" s="55"/>
-      <c r="W16" s="55"/>
-      <c r="X16" s="56"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="81"/>
+      <c r="W16" s="81"/>
+      <c r="X16" s="82"/>
     </row>
     <row r="17" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B17" s="45" t="s">
+      <c r="B17" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="46"/>
-      <c r="D17" s="46"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="47"/>
+      <c r="C17" s="72"/>
+      <c r="D17" s="72"/>
+      <c r="E17" s="72"/>
+      <c r="F17" s="73"/>
       <c r="G17" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="H17" s="48" t="s">
+      <c r="H17" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I17" s="49"/>
-      <c r="J17" s="49"/>
-      <c r="K17" s="49"/>
-      <c r="L17" s="50"/>
+      <c r="I17" s="75"/>
+      <c r="J17" s="75"/>
+      <c r="K17" s="75"/>
+      <c r="L17" s="76"/>
       <c r="M17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N17" s="51" t="s">
+      <c r="N17" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O17" s="52"/>
-      <c r="P17" s="52"/>
-      <c r="Q17" s="52"/>
-      <c r="R17" s="53"/>
+      <c r="O17" s="78"/>
+      <c r="P17" s="78"/>
+      <c r="Q17" s="78"/>
+      <c r="R17" s="79"/>
       <c r="S17" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="T17" s="54" t="s">
+      <c r="T17" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U17" s="55"/>
-      <c r="V17" s="55"/>
-      <c r="W17" s="55"/>
-      <c r="X17" s="56"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="81"/>
+      <c r="W17" s="81"/>
+      <c r="X17" s="82"/>
     </row>
     <row r="18" spans="1:24" ht="59.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="57" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="63"/>
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
       <c r="G18" s="3"/>
-      <c r="H18" s="64" t="s">
+      <c r="H18" s="60" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="65"/>
-      <c r="J18" s="65"/>
-      <c r="K18" s="65"/>
-      <c r="L18" s="66"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="61"/>
+      <c r="L18" s="62"/>
       <c r="M18" s="3"/>
-      <c r="N18" s="67" t="s">
+      <c r="N18" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="O18" s="68"/>
-      <c r="P18" s="68"/>
-      <c r="Q18" s="68"/>
-      <c r="R18" s="69"/>
+      <c r="O18" s="64"/>
+      <c r="P18" s="64"/>
+      <c r="Q18" s="64"/>
+      <c r="R18" s="65"/>
       <c r="S18" s="3"/>
-      <c r="T18" s="70" t="s">
+      <c r="T18" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="U18" s="71"/>
-      <c r="V18" s="71"/>
-      <c r="W18" s="71"/>
-      <c r="X18" s="72"/>
+      <c r="U18" s="67"/>
+      <c r="V18" s="67"/>
+      <c r="W18" s="67"/>
+      <c r="X18" s="68"/>
     </row>
     <row r="19" spans="1:24" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="45" t="s">
+      <c r="B19" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="46"/>
-      <c r="D19" s="46"/>
-      <c r="E19" s="46"/>
-      <c r="F19" s="47"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="73"/>
       <c r="G19" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="74" t="s">
         <v>14</v>
       </c>
-      <c r="I19" s="49"/>
-      <c r="J19" s="49"/>
-      <c r="K19" s="49"/>
-      <c r="L19" s="50"/>
+      <c r="I19" s="75"/>
+      <c r="J19" s="75"/>
+      <c r="K19" s="75"/>
+      <c r="L19" s="76"/>
       <c r="M19" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="N19" s="51" t="s">
+      <c r="N19" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="O19" s="52"/>
-      <c r="P19" s="52"/>
-      <c r="Q19" s="52"/>
-      <c r="R19" s="53"/>
+      <c r="O19" s="78"/>
+      <c r="P19" s="78"/>
+      <c r="Q19" s="78"/>
+      <c r="R19" s="79"/>
       <c r="S19" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="T19" s="54" t="s">
+      <c r="T19" s="80" t="s">
         <v>15</v>
       </c>
-      <c r="U19" s="55"/>
-      <c r="V19" s="55"/>
-      <c r="W19" s="55"/>
-      <c r="X19" s="56"/>
+      <c r="U19" s="81"/>
+      <c r="V19" s="81"/>
+      <c r="W19" s="81"/>
+      <c r="X19" s="82"/>
     </row>
     <row r="20" spans="1:24" ht="19.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="73" t="s">
+      <c r="B20" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="74"/>
+      <c r="C20" s="70"/>
     </row>
     <row r="21" spans="1:24" ht="21.6" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>0</v>
       </c>
-      <c r="B21" s="59" t="s">
+      <c r="B21" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="60"/>
+      <c r="C21" s="56"/>
     </row>
     <row r="22" spans="1:24" ht="19.8" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -2536,57 +2536,7 @@
     </row>
   </sheetData>
   <mergeCells count="72">
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="B10:J10"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="S6:T6"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="P4:Q4"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="P7:Q7"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:J1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="P2:Q2"/>
-    <mergeCell ref="P3:Q3"/>
-    <mergeCell ref="B2:J2"/>
-    <mergeCell ref="B3:J3"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="H18:L18"/>
-    <mergeCell ref="N18:R18"/>
-    <mergeCell ref="T18:X18"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="H17:L17"/>
-    <mergeCell ref="N17:R17"/>
-    <mergeCell ref="T17:X17"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="H19:L19"/>
-    <mergeCell ref="N19:R19"/>
-    <mergeCell ref="T19:X19"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="H15:L15"/>
-    <mergeCell ref="N15:R15"/>
-    <mergeCell ref="T15:X15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="H16:L16"/>
-    <mergeCell ref="N16:R16"/>
-    <mergeCell ref="T16:X16"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="T13:X13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="H14:L14"/>
-    <mergeCell ref="N14:R14"/>
-    <mergeCell ref="T14:X14"/>
+    <mergeCell ref="B8:J9"/>
     <mergeCell ref="B12:F12"/>
     <mergeCell ref="H12:L12"/>
     <mergeCell ref="N12:R12"/>
@@ -2603,11 +2553,61 @@
     <mergeCell ref="K8:K9"/>
     <mergeCell ref="L8:L9"/>
     <mergeCell ref="N8:N9"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="N13:R13"/>
+    <mergeCell ref="T13:X13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="H14:L14"/>
+    <mergeCell ref="N14:R14"/>
+    <mergeCell ref="T14:X14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="H15:L15"/>
+    <mergeCell ref="N15:R15"/>
+    <mergeCell ref="T15:X15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="H16:L16"/>
+    <mergeCell ref="N16:R16"/>
+    <mergeCell ref="T16:X16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="H17:L17"/>
+    <mergeCell ref="N17:R17"/>
+    <mergeCell ref="T17:X17"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="H19:L19"/>
+    <mergeCell ref="N19:R19"/>
+    <mergeCell ref="T19:X19"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="H18:L18"/>
+    <mergeCell ref="N18:R18"/>
+    <mergeCell ref="T18:X18"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:J1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="P2:Q2"/>
+    <mergeCell ref="P3:Q3"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="B3:J3"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="B10:J10"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="S6:T6"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="P7:Q7"/>
     <mergeCell ref="B4:J4"/>
     <mergeCell ref="B5:J5"/>
     <mergeCell ref="B6:J6"/>
     <mergeCell ref="B7:J7"/>
-    <mergeCell ref="B8:J9"/>
   </mergeCells>
   <phoneticPr fontId="5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2635,7 +2635,7 @@
   <dimension ref="B1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>

</xml_diff>